<commit_message>
added 2.c pow_decomp scenario, added 3.d Eratosfen bit
</commit_message>
<xml_diff>
--- a/pytester/pytester/data4test/pow/pow_result.xlsx
+++ b/pytester/pytester/data4test/pow/pow_result.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan.Vekhov\WORK\algo\AlgoOtus\pytester\pytester\data4test\pow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB37198A-D497-443D-872F-E1003CCE7DAE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7161B8-677B-4E0C-A3B0-7A83B62076B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="67">
   <si>
     <t>Algo name</t>
   </si>
@@ -170,12 +170,63 @@
   </si>
   <si>
     <t>Details</t>
+  </si>
+  <si>
+    <t>pow_bit_decomposition_2c</t>
+  </si>
+  <si>
+    <t>0.0013717</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.598379</t>
+  </si>
+  <si>
+    <t>0.0012172</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.599382</t>
+  </si>
+  <si>
+    <t>0.0012243</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.600886</t>
+  </si>
+  <si>
+    <t>0.0012155</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.601889</t>
+  </si>
+  <si>
+    <t>0.001499</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.603393</t>
+  </si>
+  <si>
+    <t>0.0013241</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.604897</t>
+  </si>
+  <si>
+    <t>0.0011735</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.606401</t>
+  </si>
+  <si>
+    <t>0.0011777</t>
+  </si>
+  <si>
+    <t>2020-02-07 14:55:01.607404</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1034,17 +1085,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1067,6 +1119,9 @@
       <c r="C2" t="s">
         <v>32</v>
       </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -1078,6 +1133,9 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1088,6 +1146,9 @@
       </c>
       <c r="C4" t="s">
         <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1100,6 +1161,9 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1111,6 +1175,9 @@
       <c r="C6" t="s">
         <v>39</v>
       </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1122,6 +1189,9 @@
       <c r="C7" t="s">
         <v>41</v>
       </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1133,6 +1203,9 @@
       <c r="C8" t="s">
         <v>43</v>
       </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1144,6 +1217,9 @@
       <c r="C9" t="s">
         <v>45</v>
       </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1154,6 +1230,9 @@
       </c>
       <c r="C10" t="s">
         <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1518,7 +1597,178 @@
         <v>31</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>